<commit_message>
route visualization working with temp coordinate data from png
</commit_message>
<xml_diff>
--- a/_extras/station_coordinates.xlsx
+++ b/_extras/station_coordinates.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="-4260" yWindow="-21600" windowWidth="38400" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="From Square" sheetId="1" r:id="rId1"/>
+    <sheet name="From Map" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,123 +20,258 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="90">
+  <si>
+    <t>Station Code</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>HY</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
   <si>
     <t>RM</t>
   </si>
   <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>EP</t>
-  </si>
-  <si>
-    <t>NB</t>
-  </si>
-  <si>
-    <t>BK</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>LM</t>
-  </si>
-  <si>
-    <t>FV</t>
-  </si>
-  <si>
-    <t>CL</t>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>SB</t>
   </si>
   <si>
     <t>SL</t>
   </si>
   <si>
-    <t>BF</t>
-  </si>
-  <si>
-    <t>HY</t>
-  </si>
-  <si>
     <t>SH</t>
   </si>
   <si>
+    <t>SS</t>
+  </si>
+  <si>
     <t>UC</t>
   </si>
   <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>CN</t>
-  </si>
-  <si>
-    <t>PH</t>
-  </si>
-  <si>
     <t>WC</t>
   </si>
   <si>
-    <t>LF</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>RR</t>
-  </si>
-  <si>
     <t>OW</t>
   </si>
   <si>
-    <t>EM</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>GP</t>
-  </si>
-  <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>WP</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>SB</t>
+    <t>HOME ORIGIN STATIONS</t>
+  </si>
+  <si>
+    <t>12th St. / Oakland City Center</t>
+  </si>
+  <si>
+    <t>16th St. Mission</t>
+  </si>
+  <si>
+    <t>19th St. / Oakland</t>
+  </si>
+  <si>
+    <t>24th St. Mission</t>
+  </si>
+  <si>
+    <t>Ashby</t>
+  </si>
+  <si>
+    <t>Balboa Park</t>
+  </si>
+  <si>
+    <t>Bay Fair</t>
+  </si>
+  <si>
+    <t>Castro Valley</t>
+  </si>
+  <si>
+    <t>Civic Center / UN Plaza</t>
+  </si>
+  <si>
+    <t>Coliseum / Oakland Airport</t>
+  </si>
+  <si>
+    <t>Colma</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>Daly City</t>
+  </si>
+  <si>
+    <t>Downtown Berkeley</t>
+  </si>
+  <si>
+    <t>Dublin / Pleasanton</t>
+  </si>
+  <si>
+    <t>El Cerrito del Norte</t>
+  </si>
+  <si>
+    <t>El Cerrito Plaza</t>
+  </si>
+  <si>
+    <t>Embarcadero</t>
+  </si>
+  <si>
+    <t>Fremont</t>
+  </si>
+  <si>
+    <t>Fruitvale</t>
+  </si>
+  <si>
+    <t>Glen Park</t>
+  </si>
+  <si>
+    <t>Hayward</t>
+  </si>
+  <si>
+    <t>Lafayette</t>
+  </si>
+  <si>
+    <t>Lake Merritt</t>
+  </si>
+  <si>
+    <t>MacArthur</t>
+  </si>
+  <si>
+    <t>Millbrae</t>
+  </si>
+  <si>
+    <t>Montgomery St.</t>
+  </si>
+  <si>
+    <t>North Berkeley</t>
+  </si>
+  <si>
+    <t>North Concord / Martinez</t>
+  </si>
+  <si>
+    <t>Orinda</t>
+  </si>
+  <si>
+    <t>Pittsburg / Bay Point</t>
+  </si>
+  <si>
+    <t>Pleasant Hill</t>
+  </si>
+  <si>
+    <t>Powell St.</t>
+  </si>
+  <si>
+    <t>Richmond</t>
+  </si>
+  <si>
+    <t>Rockridge</t>
+  </si>
+  <si>
+    <t>San Bruno</t>
+  </si>
+  <si>
+    <t>San Leandro</t>
+  </si>
+  <si>
+    <t>South Hayward</t>
+  </si>
+  <si>
+    <t>South San Francisco</t>
+  </si>
+  <si>
+    <t>Union City</t>
+  </si>
+  <si>
+    <t>Walnut Creek</t>
+  </si>
+  <si>
+    <t>West Oakland</t>
   </si>
   <si>
     <t>SO</t>
   </si>
   <si>
-    <t>MB</t>
+    <t>San Francisco Airport</t>
   </si>
   <si>
     <t>st_id</t>
@@ -145,16 +281,48 @@
   </si>
   <si>
     <t>y_axis</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,14 +352,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -521,33 +694,1018 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="400" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <f>C43+1</f>
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <f>D43</f>
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <f>C5+1</f>
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <f>D5-1</f>
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <f>C2</f>
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <f>D2-1</f>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <f>C22+1</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f>D22-1</f>
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <f>C26-1</f>
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <f>D26-1</f>
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <f>C14+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <f>D14-1</f>
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <f>C38+1</f>
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <f>D28+1</f>
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9">
+        <f>C8+1</f>
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <f>D8</f>
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <f>C3+1</f>
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <f>D3-1</f>
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <f>C21+1</f>
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <f>D21+1</f>
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <f>C14+1</f>
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f>D14+1</f>
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <f>C33+1</f>
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <f>D33-1</f>
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <f>C6-1</f>
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <f>D6-1</f>
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16">
+        <f>C9+1</f>
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <f>D9</f>
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17">
+        <f>C18-1</f>
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <f>D18-1</f>
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <f>C29-1</f>
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <f>D29-1</f>
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19">
+        <f>C28+1</f>
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <f>D28-1</f>
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20">
+        <f>C41+1</f>
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <f>D41+1</f>
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21">
+        <f>C25+1</f>
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <f>D25+1</f>
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <f>C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f>D7-1</f>
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23">
+        <f>C8+1</f>
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <f>D8+1</f>
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24">
+        <f>C31+1</f>
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <f>D31-1</f>
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25">
+        <f>C2</f>
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <f>D2+1</f>
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <f>C4</f>
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <f>D4-1</f>
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27">
+        <f>C37+1</f>
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <f>D37+1</f>
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28">
+        <f>C34+1</f>
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <f>D34-1</f>
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29">
+        <f>C15-1</f>
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <f>D15-1</f>
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30">
+        <f>C13+1</f>
+        <v>23</v>
+      </c>
+      <c r="D30">
+        <f>D13-1</f>
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31">
+        <f>C36+1</f>
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <f>D36-1</f>
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32">
+        <f>C30+1</f>
+        <v>24</v>
+      </c>
+      <c r="D32">
+        <f>D30-1</f>
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33">
+        <f>C42+1</f>
+        <v>21</v>
+      </c>
+      <c r="D33">
+        <f>D42-1</f>
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34">
+        <f>C10+1</f>
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <f>D10-1</f>
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35">
+        <f>C17-1</f>
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <f>D17-1</f>
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36">
+        <f>C26+1</f>
+        <v>17</v>
+      </c>
+      <c r="D36">
+        <f>D26-1</f>
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37">
+        <f>C40+1</f>
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <f>D40+1</f>
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
+        <f>C11+1</f>
+        <v>19</v>
+      </c>
+      <c r="D38">
+        <f>D11+1</f>
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39">
+        <f>C23+1</f>
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <f>D23+1</f>
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40">
+        <f>C12+1</f>
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <f>D12+1</f>
+        <v>23</v>
+      </c>
+      <c r="E40" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41">
+        <f>C39+1</f>
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <f>D39+1</f>
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42">
+        <f>C24+1</f>
+        <v>20</v>
+      </c>
+      <c r="D42">
+        <f>D24-1</f>
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="2">
+        <f>15</f>
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <f>D19</f>
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44">
+        <f>C37+1</f>
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <f>D37</f>
+        <v>24</v>
+      </c>
+      <c r="E44" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>468</v>
@@ -558,7 +1716,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>481</v>
@@ -569,7 +1727,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>503</v>
@@ -580,7 +1738,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>525</v>
@@ -591,7 +1749,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>543</v>
@@ -602,7 +1760,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>560</v>
@@ -613,7 +1771,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>574</v>
@@ -646,7 +1804,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>600</v>
@@ -657,18 +1815,18 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>631</v>
       </c>
       <c r="C12">
-        <v>998</v>
+        <v>498</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>665</v>
@@ -679,7 +1837,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>694</v>
@@ -690,7 +1848,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>728</v>
@@ -701,7 +1859,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>793</v>
@@ -712,7 +1870,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>837</v>
@@ -723,7 +1881,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>895</v>
@@ -745,7 +1903,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>895</v>
@@ -756,7 +1914,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>842</v>
@@ -767,7 +1925,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>786</v>
@@ -789,7 +1947,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>675</v>
@@ -800,7 +1958,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <v>623</v>
@@ -811,7 +1969,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>502</v>
@@ -822,7 +1980,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>410</v>
@@ -833,7 +1991,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <v>400</v>
@@ -844,7 +2002,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B29">
         <v>388</v>
@@ -855,7 +2013,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B30">
         <v>379</v>
@@ -888,7 +2046,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>340</v>
@@ -899,7 +2057,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B34">
         <v>320</v>
@@ -910,7 +2068,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B35">
         <v>306</v>
@@ -921,7 +2079,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B36">
         <v>301</v>
@@ -932,7 +2090,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B37">
         <v>832</v>
@@ -943,7 +2101,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B38">
         <v>936</v>
@@ -954,7 +2112,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B39">
         <v>954</v>
@@ -965,7 +2123,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B40">
         <v>1008</v>
@@ -987,7 +2145,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B42">
         <v>347</v>
@@ -998,7 +2156,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="B43">
         <v>405</v>
@@ -1009,7 +2167,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B44">
         <v>414</v>

</xml_diff>